<commit_message>
Excel to datagrid is changed
</commit_message>
<xml_diff>
--- a/Cp2DevExPrh/Cp2DevExPrh/File/Puanlama.xlsx
+++ b/Cp2DevExPrh/Cp2DevExPrh/File/Puanlama.xlsx
@@ -400,7 +400,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
statistics page is added
</commit_message>
<xml_diff>
--- a/Cp2DevExPrh/Cp2DevExPrh/File/Puanlama.xlsx
+++ b/Cp2DevExPrh/Cp2DevExPrh/File/Puanlama.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Puanlama" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>KullaniciAdi</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Puan</t>
   </si>
   <si>
-    <t>Burak Simsek</t>
+    <t>Mustafa Tikir</t>
   </si>
   <si>
     <t>hasbabalar@gmail.com</t>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>BurgerKing</t>
-  </si>
-  <si>
-    <t>Mustafa Tikir</t>
   </si>
 </sst>
 </file>
@@ -100,8 +97,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="KullaniciAdi"/>
     <tableColumn id="2" name="KullaniciMaili"/>
@@ -397,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="6.140625" customWidth="1"/>
@@ -436,7 +433,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,35 +447,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>